<commit_message>
Completed all the compile time tests for all math functions, now just have to insert the data into excel.
</commit_message>
<xml_diff>
--- a/Math Function Compile Time Results & Data.xlsx
+++ b/Math Function Compile Time Results & Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Empty Scene</t>
   </si>
@@ -33,6 +33,45 @@
   </si>
   <si>
     <t>COMPILE TIMES OF VARIOUS MATH FUNCTIONS IN UNITY</t>
+  </si>
+  <si>
+    <t>No Data</t>
+  </si>
+  <si>
+    <t>Low Value</t>
+  </si>
+  <si>
+    <t>High Value</t>
+  </si>
+  <si>
+    <t>Clamp Function</t>
+  </si>
+  <si>
+    <t>Approximately Function</t>
+  </si>
+  <si>
+    <t>DeltaAngle Function</t>
+  </si>
+  <si>
+    <t>Lerp Function</t>
+  </si>
+  <si>
+    <t>LerpUnclamped Function</t>
+  </si>
+  <si>
+    <t>MoveTowards Function</t>
+  </si>
+  <si>
+    <t>LookAt Function</t>
+  </si>
+  <si>
+    <t>SmoothDamp Function</t>
+  </si>
+  <si>
+    <t>Log Function</t>
+  </si>
+  <si>
+    <t>Random Function</t>
   </si>
 </sst>
 </file>
@@ -84,17 +123,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,173 +421,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M24"/>
+  <dimension ref="C2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="3:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D4" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="1">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="1">
-        <v>4</v>
-      </c>
       <c r="H5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
         <v>6</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>7</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>8</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>9</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>2.62</v>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E6">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F6">
         <v>2.64</v>
       </c>
-      <c r="F6">
-        <v>2.77</v>
-      </c>
       <c r="G6">
-        <v>2.63</v>
+        <v>2.84</v>
       </c>
       <c r="H6">
-        <v>2.66</v>
+        <v>2.89</v>
       </c>
       <c r="I6">
-        <v>2.64</v>
+        <v>2.92</v>
       </c>
       <c r="J6">
-        <v>3.02</v>
+        <v>2.69</v>
       </c>
       <c r="K6">
-        <v>2.63</v>
+        <v>2.8</v>
       </c>
       <c r="L6">
-        <v>2.69</v>
+        <v>3.03</v>
       </c>
       <c r="M6">
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
+        <v>2.67</v>
+      </c>
+      <c r="N6">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D4:M4"/>
-    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="E4:N4"/>
+    <mergeCell ref="D2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>